<commit_message>
adding phase 1 task evidence
</commit_message>
<xml_diff>
--- a/beal2912/evidence.xlsx
+++ b/beal2912/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18197" windowHeight="8503"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18197" windowHeight="8503" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="75">
   <si>
     <t>TxHash</t>
   </si>
@@ -161,6 +161,108 @@
   </si>
   <si>
     <t>iaa1rxftqkksy3u6n4sdu6l9mz30vm72n9l4uhzdj4</t>
+  </si>
+  <si>
+    <t>9D22030DAF25B56948A0264143F61441D9A4B1696B0927B011DE3AAA33BDDBEF</t>
+  </si>
+  <si>
+    <t>beal01</t>
+  </si>
+  <si>
+    <t>84ED37357037D6CF25C5242D53D1CE3900510CAE2D8E624B26FE135102C0D62C</t>
+  </si>
+  <si>
+    <t>bnft1</t>
+  </si>
+  <si>
+    <t>DBC9F1B4C05C17ACD97B4AFB6FCE179DE05E4F16A3D5D90EA3A67F44780B3D8A</t>
+  </si>
+  <si>
+    <t>bnft2</t>
+  </si>
+  <si>
+    <t>0BA03D40893A3D8296960976FE7D4812EFF8BE14DDED084C390A7DB63872037C</t>
+  </si>
+  <si>
+    <t>error while trying to make a duplicate nft</t>
+  </si>
+  <si>
+    <t>C1AFB0452176191331E85FAE7447D209FC7B7186994BDD076C1B21C334358E98</t>
+  </si>
+  <si>
+    <t>DBD13778AE5B355F294682AE6F3A93822A00483C0AB2C3B18D73C034D752516B</t>
+  </si>
+  <si>
+    <t>37C83299B246EA9A6438C83B13C2AAB1447DF68BDD8A376A9900CE232FB8B7BA</t>
+  </si>
+  <si>
+    <t>juno1a26q7r8rkf8zrlt3wcdwx3vc4vzwc7kjf4vryjxh3hx5rkjuq8ds8nw5wa</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>F9D9E91A3192BE0AEAA880A4D4E35BD354CE2A5CFA348DF286A37B92EE7AAEF2</t>
+  </si>
+  <si>
+    <t>bnft3</t>
+  </si>
+  <si>
+    <t>CB215CB0395376AC92ADF7F35DD8302940F5BE959AA2B930AEF189038327AABD</t>
+  </si>
+  <si>
+    <t>bnft4</t>
+  </si>
+  <si>
+    <t>C680BC4EAB1B393B2EBDE1E6A8B13528C331682C6E98951DF37B27B3E9AC6AAA</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>31C78F04CE79F5A25E38944C556D094E8E5DE4EDF2CCB5C489C9587DEF7F45C8</t>
+  </si>
+  <si>
+    <t>1st try on channel-0, reverted I don't know why</t>
+  </si>
+  <si>
+    <t>ibc/332EF1AB47C63F94D5053C3C8A2360AC65B58EDD1D689F88443BCFE0BCD6BF70</t>
+  </si>
+  <si>
+    <t>2nd try on channel-1 -&gt; OK</t>
+  </si>
+  <si>
+    <t>5EA2372D36DB62D7584199B34CBD11B5DB9AFBD6A33A1C869BA2B20AACFC7BD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gon-irishub-1</t>
+  </si>
+  <si>
+    <t>210F614FEB94D3E7B6BD85C88F034B0A0D82EE9505DD29F2FF9848F8C01F5650</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>962007845F1DB9B2BCCBF5A9257028E21F16702E797B8D781E5575E6E48E75D5</t>
+  </si>
+  <si>
+    <t>stars1p5uwda7k7cynglf6mzux63hvm0zp5tpcm06dugjfn3lc99elpmzqzs2zrn</t>
+  </si>
+  <si>
+    <t>KO first try, Juno account wasn't set up, tx reverted</t>
+  </si>
+  <si>
+    <t>KO try on channel 13</t>
+  </si>
+  <si>
+    <t>OK try on channel 24</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>6FF131EFB497F644DF3CCB76C34447F3D7D4E5B0AF2DF22B1CAABF7D844D1845</t>
   </si>
 </sst>
 </file>
@@ -234,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -250,6 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,8 +657,8 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1090,13 +1193,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="2" width="17.84375" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="70.07421875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="63.3828125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1113,6 +1219,14 @@
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1357,17 +1471,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="2" width="17.84375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="69.69140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.84375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.921875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1378,7 +1496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1389,6 +1507,58 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1399,18 +1569,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="2" width="17.84375" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A24:A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="69" style="3" customWidth="1"/>
+    <col min="2" max="2" width="81.69140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1438,6 +1611,59 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1448,18 +1674,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="2" width="17.84375" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="75.07421875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="71.23046875" style="3" customWidth="1"/>
     <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1473,7 +1702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1487,6 +1716,37 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1497,18 +1757,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="2" width="17.84375" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="68.07421875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="64.23046875" style="3" customWidth="1"/>
     <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1522,7 +1785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1536,6 +1799,40 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1546,14 +1843,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="17.84375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="69.53515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="72.15234375" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.3046875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.4609375" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -1586,6 +1885,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edit info format, + remove extra line on A3,A4,A5,A6
</commit_message>
<xml_diff>
--- a/beal2912/evidence.xlsx
+++ b/beal2912/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18197" windowHeight="8503" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18197" windowHeight="8503" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="124">
   <si>
     <t>TxHash</t>
   </si>
@@ -82,30 +82,6 @@
     <t>Community</t>
   </si>
   <si>
-    <t>team name</t>
-  </si>
-  <si>
-    <t>addr1</t>
-  </si>
-  <si>
-    <t>addr2</t>
-  </si>
-  <si>
-    <t>addr3</t>
-  </si>
-  <si>
-    <t>addr4</t>
-  </si>
-  <si>
-    <t>addr5</t>
-  </si>
-  <si>
-    <t>discord#1234</t>
-  </si>
-  <si>
-    <t>set none if no community</t>
-  </si>
-  <si>
     <t>beal2912</t>
   </si>
   <si>
@@ -136,24 +112,6 @@
     <t>beal01</t>
   </si>
   <si>
-    <t>84ED37357037D6CF25C5242D53D1CE3900510CAE2D8E624B26FE135102C0D62C</t>
-  </si>
-  <si>
-    <t>bnft1</t>
-  </si>
-  <si>
-    <t>DBC9F1B4C05C17ACD97B4AFB6FCE179DE05E4F16A3D5D90EA3A67F44780B3D8A</t>
-  </si>
-  <si>
-    <t>bnft2</t>
-  </si>
-  <si>
-    <t>37C83299B246EA9A6438C83B13C2AAB1447DF68BDD8A376A9900CE232FB8B7BA</t>
-  </si>
-  <si>
-    <t>juno1a26q7r8rkf8zrlt3wcdwx3vc4vzwc7kjf4vryjxh3hx5rkjuq8ds8nw5wa</t>
-  </si>
-  <si>
     <t>uni-6</t>
   </si>
   <si>
@@ -181,9 +139,6 @@
     <t>5EA2372D36DB62D7584199B34CBD11B5DB9AFBD6A33A1C869BA2B20AACFC7BD2</t>
   </si>
   <si>
-    <t xml:space="preserve"> gon-irishub-1</t>
-  </si>
-  <si>
     <t>210F614FEB94D3E7B6BD85C88F034B0A0D82EE9505DD29F2FF9848F8C01F5650</t>
   </si>
   <si>
@@ -194,9 +149,6 @@
   </si>
   <si>
     <t>stars1p5uwda7k7cynglf6mzux63hvm0zp5tpcm06dugjfn3lc99elpmzqzs2zrn</t>
-  </si>
-  <si>
-    <t>6FF131EFB497F644DF3CCB76C34447F3D7D4E5B0AF2DF22B1CAABF7D844D1845</t>
   </si>
   <si>
     <t>bnft5</t>
@@ -479,7 +431,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,11 +441,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -531,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -541,9 +488,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -857,10 +801,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -869,7 +813,7 @@
     <col min="2" max="2" width="41.61328125" style="3" customWidth="1"/>
     <col min="3" max="3" width="44.61328125" style="3" customWidth="1"/>
     <col min="4" max="4" width="44.53515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="51.765625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="51.765625" style="5" customWidth="1"/>
     <col min="6" max="6" width="52.84375" style="3" customWidth="1"/>
     <col min="7" max="7" width="14.53515625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
@@ -901,56 +845,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>17</v>
+      <c r="B2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -985,42 +903,42 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>63</v>
+      <c r="A5" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
-        <v>64</v>
+      <c r="A6" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1035,8 +953,8 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1055,42 +973,42 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>69</v>
+      <c r="A5" s="6" t="s">
+        <v>53</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
-        <v>70</v>
+      <c r="A6" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1125,58 +1043,58 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="7" t="s">
-        <v>73</v>
+      <c r="A6" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
-        <v>74</v>
+      <c r="A7" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" s="7" t="s">
-        <v>75</v>
+      <c r="A8" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1211,58 +1129,58 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="9" t="s">
-        <v>76</v>
+      <c r="A3" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1297,34 +1215,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>89</v>
+      <c r="A5" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1359,34 +1277,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>97</v>
+      <c r="A5" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1421,34 +1339,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>101</v>
+      <c r="A5" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -1486,34 +1404,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>111</v>
+      <c r="A5" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1548,34 +1466,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>120</v>
+      <c r="A5" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1610,34 +1528,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>125</v>
+      <c r="A5" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1653,7 +1571,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1672,10 +1590,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1710,50 +1628,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>130</v>
+      <c r="A5" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
-        <v>132</v>
+      <c r="A6" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="10" t="s">
-        <v>131</v>
+      <c r="A7" s="9" t="s">
+        <v>115</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1788,50 +1706,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
-        <v>137</v>
+      <c r="A5" s="9" t="s">
+        <v>121</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
-        <v>138</v>
+      <c r="A6" s="9" t="s">
+        <v>122</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="10" t="s">
-        <v>139</v>
+      <c r="A7" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1846,11 +1764,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.15234375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1980,10 +1900,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2005,89 +1925,89 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>33</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>35</v>
+      <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="8" t="s">
-        <v>56</v>
+      <c r="A6" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>65</v>
@@ -2095,123 +2015,101 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A18" s="4" t="s">
-        <v>121</v>
+      <c r="A18" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A19" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A20" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2224,10 +2122,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2252,36 +2150,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>38</v>
+      <c r="C2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="E4" s="7"/>
+      <c r="E3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2296,7 +2180,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2323,16 +2207,16 @@
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -2351,7 +2235,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2378,31 +2262,19 @@
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -2420,8 +2292,8 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2448,16 +2320,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2492,34 +2364,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>53</v>
+      <c r="A5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2554,34 +2426,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>62</v>
+      <c r="A5" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction on A7 to A12 and adding B5 to B7
</commit_message>
<xml_diff>
--- a/beal2912/evidence.xlsx
+++ b/beal2912/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18197" windowHeight="8503" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18197" windowHeight="8503" tabRatio="620" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -32,23 +32,18 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="115">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -163,45 +158,27 @@
     <t>2865E8773B01B9C4EC77B3B87A5F2FA5FB5FD05F27CA4BA9F431C15913488B50</t>
   </si>
   <si>
-    <t>juno1gk93fzq52chgj25pft2fvpkayuj9a4xwp0w9ghh2cvpmksq43ktq4usce2</t>
-  </si>
-  <si>
     <t>ibc/0B6B124BE0862A7CB0B6DB16B8FD068C1A5831B2A80B277236F82A6A76A86A46</t>
   </si>
   <si>
-    <t>ibc/C29C6A942CB9DCC48A1446521769371550446AB7BCFAC294AD0FF4D909625C8C</t>
-  </si>
-  <si>
-    <t>ibc/075A8AFE2832E0887BE0660703EE7B1CA34849C79CBE87352C166D93ACADE015</t>
-  </si>
-  <si>
     <t>bnft7</t>
   </si>
   <si>
     <t>ibc/5140544D21A0099115393B0EFC3B9829F334674F1D839C6BCFDDC14D914D44DD</t>
   </si>
   <si>
-    <t>ibc/782F27264DA520AC9DC96E6E90CB433AEC9D648D989361BD491FA037BA5B6F6C</t>
-  </si>
-  <si>
     <t>ibc/DE7FC6B4882357EA10E20334381689CA6121A9A0E48554A7AF1B5062F25FA3D2</t>
   </si>
   <si>
     <t>bnft8</t>
   </si>
   <si>
-    <t>ibc/7684F6F33DDE03EFA8902F48AADEA4EF95343D590E68DDC406FFBFD412AAFDA7</t>
-  </si>
-  <si>
     <t>C889723D172FC6908A8B7C67C67A8474FC9E8E55503AB5EFA5E4D9FE9F3FB21C</t>
   </si>
   <si>
     <t>7E90F86D959D28A590775A086971D0456368D2F8C389340713EE75417F868D55</t>
   </si>
   <si>
-    <t>juno1m7rfwn5ruk2lp40ea94rnkl7qhvfhph38qvnn6rpqjwzglm9xh2stcccmc</t>
-  </si>
-  <si>
     <t>ibc/C82994C965AEBF09D1185B0056ABD370090309959FB4869E4D168AB977982FCE</t>
   </si>
   <si>
@@ -211,36 +188,15 @@
     <t>7DF96C8DD4CD4D2E7C8D8BF0708396144F7E8A2DA7DE2E6CA123574FAC1371CF</t>
   </si>
   <si>
-    <t>ibc/248EB44EAB36081AF8BC380997FCE6016C48844591505742DE981C1DEEDEFECE</t>
-  </si>
-  <si>
-    <t>stars1r9rnckrsg7hnr0feaf9kh5s4cgxvuqfun0d69c0q0c4q8wfpapwqwteqr9</t>
-  </si>
-  <si>
     <t>ibc/DEBB211C73A15F697258E01E1320E7952B251E11338C621BF16238149CDAFFD7</t>
   </si>
   <si>
-    <t>ibc/7D7684659397423B81A886590E7E18C9315434C704A8A561C67E5270F2A130DB</t>
-  </si>
-  <si>
-    <t>stars1j0ng7mcz5v33fnrn7y34zsza3wg6y4g9lwjhcv22yj32dqsfhfmqlppsx5</t>
-  </si>
-  <si>
-    <t>ibc/C1553FBDFF967B58FE77127157FA24D325EA3C63C5259802F63C89F8EF0FD316</t>
-  </si>
-  <si>
-    <t>ibc/8776354294FC86883F3577C71017D95EC003F7C3FDEFD17FEAFF68CC8C9BCBC0</t>
-  </si>
-  <si>
     <t>5767003C778D2FB08065D9304EC444C77DB16FBD3CE4E3573D9B3E4532C0126B</t>
   </si>
   <si>
     <t>bnft11</t>
   </si>
   <si>
-    <t>juno1h6tg32pe0t0uh9m7437nuqrxyvutd6kntsf7yhml0tze5uvc4dzqags5d0</t>
-  </si>
-  <si>
     <t>ibc/D68C6D601E5DB8A2DDBEE2FA3C2244C60CEF83641DBD95533BF4D342E0CFB91C</t>
   </si>
   <si>
@@ -410,6 +366,24 @@
   </si>
   <si>
     <t>965A0AA3FAD89AC13613DB65471C606E0CF8BAB8D6A5A0D6736D5A02706FC6E7</t>
+  </si>
+  <si>
+    <t>B642BE9AE62539E5AA65A21CFFE6AC776C02300951C12F82DB40662A9AC4AE35</t>
+  </si>
+  <si>
+    <t>50AF9497BC4D8EF160DAD000568A7193E03C911A957B7FF3575AF483D0564B48</t>
+  </si>
+  <si>
+    <t>6FFDA438AEAE41B592CE815F3E7FD908B05FE239710120219EFA71825D77143B</t>
+  </si>
+  <si>
+    <t>3B2541EAF71814DB6B6B23D6B5E7DF7D595F6EDA8B0257AC6BC056384213F592</t>
+  </si>
+  <si>
+    <t>44C4FC80A9EB21AEFF940E24841521124FE158473A4855BD1414A1BB85EA24B4</t>
+  </si>
+  <si>
+    <t>22405D2234649FFA1D2715ADE0B78B05CB7CAB4928A796FC8BAFCCF31FE969F6</t>
   </si>
 </sst>
 </file>
@@ -478,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -493,9 +467,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -821,55 +792,55 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -881,10 +852,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -895,50 +866,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>45</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -951,10 +890,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -965,50 +904,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1021,10 +928,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1035,160 +942,253 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="74" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.61328125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="80.53515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.15234375" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.45" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="76.765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.53515625" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>47</v>
+      <c r="A5" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="74" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.61328125" style="3" customWidth="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="80.3046875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.15234375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
-        <v>62</v>
+      <c r="A5" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="B6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1196,13 +1196,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="80.53515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.15234375" style="3" customWidth="1"/>
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="82.3046875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1210,77 +1210,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="76.765625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.53515625" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -1288,45 +1226,45 @@
         <v>79</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="80.3046875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.15234375" style="3" customWidth="1"/>
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="81.765625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1334,50 +1272,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
-        <v>85</v>
+      <c r="A5" s="8" t="s">
+        <v>89</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B6" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1385,13 +1320,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="82.3046875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="87.3828125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27.15234375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1399,23 +1334,23 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -1423,36 +1358,74 @@
         <v>93</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
-        <v>95</v>
+      <c r="A5" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="81.765625" style="3" customWidth="1"/>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="70.07421875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="63.3828125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="81.61328125" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1461,61 +1434,77 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
-        <v>104</v>
+      <c r="A5" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="87.3828125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.15234375" style="3" customWidth="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="82.07421875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.4609375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1523,371 +1512,224 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
+      <c r="B7" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="41.15234375" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="70.07421875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="63.3828125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="81.61328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.4609375" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="82.07421875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.4609375" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="41.15234375" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="16.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="12.4609375" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1919,197 +1761,197 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2141,27 +1983,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -2196,27 +2038,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -2251,27 +2093,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -2309,27 +2151,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -2342,10 +2184,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2356,42 +2198,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>37</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2404,10 +2222,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2418,42 +2236,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>